<commit_message>
fixing error when all observations in the aggregating groups are NA. previously sum(na.rm=T) will return 0, now it will be na.
</commit_message>
<xml_diff>
--- a/Output/2023/116-17.18.3-1592-SG_STT_NSDSFDGVT-1132.xlsx
+++ b/Output/2023/116-17.18.3-1592-SG_STT_NSDSFDGVT-1132.xlsx
@@ -2752,7 +2752,7 @@
         <v>2022</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H12" t="n">
         <v>2022</v>
@@ -3102,7 +3102,7 @@
         <v>2022</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H19" t="n">
         <v>2022</v>
@@ -3152,7 +3152,7 @@
         <v>2022</v>
       </c>
       <c r="G20" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H20" t="n">
         <v>2022</v>
@@ -3302,7 +3302,7 @@
         <v>2022</v>
       </c>
       <c r="G23" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H23" t="n">
         <v>2022</v>
@@ -17202,7 +17202,7 @@
         <v>2021</v>
       </c>
       <c r="G301" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H301" t="n">
         <v>2021</v>
@@ -17252,7 +17252,7 @@
         <v>2021</v>
       </c>
       <c r="G302" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H302" t="n">
         <v>2021</v>
@@ -31352,7 +31352,7 @@
         <v>2020</v>
       </c>
       <c r="G584" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H584" t="n">
         <v>2020</v>
@@ -31402,7 +31402,7 @@
         <v>2020</v>
       </c>
       <c r="G585" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="H585" t="n">
         <v>2020</v>

</xml_diff>